<commit_message>
Deleted and reuploaded voxelVolumes_treatment file despite obsolete usage given current Normalization.py output
</commit_message>
<xml_diff>
--- a/Statistical Analysis/voxelVolumes_treatments.xlsx
+++ b/Statistical Analysis/voxelVolumes_treatments.xlsx
@@ -1,31 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pradneshkolluru/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Education School/Duke University/Year 4 (2022-2023)/Courses/Semester 1/BME 493 (Badea Independent Study)/Bass-Connections-F22/Statistical Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4503B147-06E3-3B4B-B653-6980F0902D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5094BE39-35FC-6C41-8DA0-4B4A362B7E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4300" yWindow="2700" windowWidth="27640" windowHeight="16940" xr2:uid="{AE57A1BD-B443-BE45-BD32-84EAF64FA261}"/>
+    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="voxelVolumes_treatments" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -967,8 +962,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -976,16 +971,316 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -993,15 +1288,204 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="4" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="5" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="6" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="7" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="8" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="9" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="10" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="11" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="12" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="13" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="14" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="15" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="16" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="17" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="18" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="20" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="21" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="22" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="23" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="24" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="28" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="29" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="30" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="31" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="32" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="33" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="34" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="35" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="36" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="37" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="38" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="39" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1312,12 +1796,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59FDFEE5-B409-C545-B402-9F1DB0D336F1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD26"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -21342,6 +21824,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>